<commit_message>
Added vrsta ograje (balkonska)
</commit_message>
<xml_diff>
--- a/bin/Debug/TemplateVodoravne.xlsx
+++ b/bin/Debug/TemplateVodoravne.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timpo\OneDrive\Namizje\GivosApp\GivosCalc\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FDD9D6-CD4D-4ABC-B14E-587C0D1F1AE7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA45BDD-DC67-4693-8F60-CE97AC923ADF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Z montažo" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="65">
   <si>
     <t>DATUM :</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>POPUST</t>
+  </si>
+  <si>
+    <t>POKROV</t>
   </si>
 </sst>
 </file>
@@ -784,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1205,7 +1208,9 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
+      <c r="A39" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="B39" s="15" t="s">
         <v>28</v>
       </c>
@@ -1444,8 +1449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1865,7 +1870,9 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
+      <c r="A39" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="B39" s="15" t="s">
         <v>28</v>
       </c>

</xml_diff>